<commit_message>
updated body et al.
</commit_message>
<xml_diff>
--- a/Data/Placement.xlsx
+++ b/Data/Placement.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bomeara/Documents/MyDocuments/GitClones/EEB_NRT/Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="18040" yWindow="2200" windowWidth="15560" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -65,10 +60,10 @@
     <t>FWF PhD</t>
   </si>
   <si>
-    <t>Enrolled in  PhD program</t>
-  </si>
-  <si>
     <t>FWF Masters</t>
+  </si>
+  <si>
+    <t>Active PhD student</t>
   </si>
 </sst>
 </file>
@@ -163,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -198,7 +193,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -375,7 +370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -386,15 +381,15 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,10 +406,10 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -434,7 +429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -454,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -474,7 +469,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -494,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -514,7 +509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -534,9 +529,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -554,7 +549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -576,5 +571,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>